<commit_message>
the tag wall is now working
a couple changes to come
</commit_message>
<xml_diff>
--- a/goOut/HashTag Mappings.xlsx
+++ b/goOut/HashTag Mappings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>HashTag Groupings</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Can'tHearMyselfTalk</t>
+  </si>
+  <si>
+    <t>People</t>
   </si>
 </sst>
 </file>
@@ -532,7 +535,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +569,9 @@
       <c r="E3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>